<commit_message>
fixbug: lacking line table; add pre_login_time for user
</commit_message>
<xml_diff>
--- a/数据库/db.xlsx
+++ b/数据库/db.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="130">
   <si>
     <t>用户表-user</t>
   </si>
@@ -67,16 +67,22 @@
     <t>default '无名'</t>
   </si>
   <si>
+    <t>pre_login_time</t>
+  </si>
+  <si>
+    <t>用户上次登录时间</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>not null default now()</t>
+  </si>
+  <si>
     <t>signup_time</t>
   </si>
   <si>
     <t>用户注册时间</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>not null default now()</t>
   </si>
   <si>
     <t>token</t>
@@ -421,12 +427,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -439,16 +451,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -465,16 +477,16 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -495,6 +507,7 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff4c4c4c"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -694,17 +707,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -728,14 +741,14 @@
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:srgbClr val="4C4C4C"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -983,12 +996,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1275,7 +1288,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1299,14 +1312,14 @@
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:srgbClr val="4C4C4C"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1557,7 +1570,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1665,87 +1678,89 @@
         <v>23</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>24</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="D7" t="s" s="4">
+        <v>21</v>
+      </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" ht="15" customHeight="1">
       <c r="A8" t="s" s="4">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s" s="4">
         <v>25</v>
       </c>
-      <c r="B8" t="s" s="4">
+      <c r="C8" t="s" s="4">
         <v>26</v>
       </c>
-      <c r="C8" t="s" s="4">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" t="s" s="4">
         <v>27</v>
       </c>
-      <c r="D8" t="s" s="4">
+      <c r="B9" t="s" s="4">
         <v>28</v>
       </c>
-      <c r="E8" t="s" s="4">
+      <c r="C9" t="s" s="4">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="D9" t="s" s="4">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s" s="4">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" ht="15" customHeight="1">
-      <c r="A11" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E11" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A11" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" ht="15" customHeight="1">
       <c r="A12" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s" s="4">
-        <v>32</v>
-      </c>
-      <c r="E12" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E12" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" ht="15" customHeight="1">
       <c r="A13" t="s" s="4">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s" s="4">
         <v>33</v>
       </c>
-      <c r="B13" t="s" s="4">
+      <c r="C13" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s" s="4">
         <v>34</v>
       </c>
-      <c r="C13" t="s" s="4">
-        <v>16</v>
-      </c>
-      <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
     <row r="14" ht="15" customHeight="1">
@@ -1756,72 +1771,72 @@
         <v>36</v>
       </c>
       <c r="C14" t="s" s="4">
+        <v>16</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" ht="15" customHeight="1">
+      <c r="A15" t="s" s="4">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s" s="4">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="D14" t="s" s="4">
-        <v>28</v>
-      </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="D15" t="s" s="4">
+        <v>30</v>
+      </c>
       <c r="E15" s="5"/>
     </row>
     <row r="16" ht="15" customHeight="1">
-      <c r="A16" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" ht="15" customHeight="1">
-      <c r="A17" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D17" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E17" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A17" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" ht="15" customHeight="1">
       <c r="A18" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D18" t="s" s="4">
-        <v>32</v>
-      </c>
-      <c r="E18" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E18" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" ht="15" customHeight="1">
       <c r="A19" t="s" s="4">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s" s="4">
         <v>33</v>
       </c>
-      <c r="B19" t="s" s="4">
+      <c r="C19" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s" s="4">
         <v>34</v>
       </c>
-      <c r="C19" t="s" s="4">
-        <v>16</v>
-      </c>
-      <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" ht="15" customHeight="1">
@@ -1829,28 +1844,26 @@
         <v>35</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s" s="4">
-        <v>28</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
     <row r="21" ht="15" customHeight="1">
       <c r="A21" t="s" s="4">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s" s="4">
         <v>40</v>
       </c>
       <c r="C21" t="s" s="4">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s" s="4">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E21" s="5"/>
     </row>
@@ -1862,19 +1875,27 @@
         <v>42</v>
       </c>
       <c r="C22" t="s" s="4">
+        <v>16</v>
+      </c>
+      <c r="D22" t="s" s="4">
+        <v>13</v>
+      </c>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" ht="15" customHeight="1">
+      <c r="A23" t="s" s="4">
         <v>43</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" ht="15" customHeight="1">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="B23" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s" s="4">
+        <v>45</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" ht="12.75" customHeight="1" hidden="1">
+    <row r="24" ht="15" customHeight="1">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1895,50 +1916,42 @@
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" ht="15" customHeight="1">
-      <c r="A27" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+    <row r="27" ht="12.75" customHeight="1" hidden="1">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" ht="15" customHeight="1">
-      <c r="A28" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D28" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E28" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A28" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
     </row>
     <row r="29" ht="15" customHeight="1">
       <c r="A29" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D29" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E29" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E29" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" ht="15" customHeight="1">
       <c r="A30" t="s" s="4">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s" s="4">
         <v>47</v>
@@ -1947,37 +1960,37 @@
         <v>8</v>
       </c>
       <c r="D30" t="s" s="4">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="E30" s="5"/>
     </row>
     <row r="31" ht="15" customHeight="1">
       <c r="A31" t="s" s="4">
+        <v>48</v>
+      </c>
+      <c r="B31" t="s" s="4">
         <v>49</v>
-      </c>
-      <c r="B31" t="s" s="4">
-        <v>50</v>
       </c>
       <c r="C31" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D31" t="s" s="4">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E31" s="5"/>
     </row>
     <row r="32" ht="15" customHeight="1">
       <c r="A32" t="s" s="4">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s" s="4">
         <v>52</v>
       </c>
-      <c r="B32" t="s" s="4">
+      <c r="C32" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s" s="4">
         <v>53</v>
-      </c>
-      <c r="C32" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="D32" t="s" s="4">
-        <v>21</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -1991,7 +2004,9 @@
       <c r="C33" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="D33" s="5"/>
+      <c r="D33" t="s" s="4">
+        <v>21</v>
+      </c>
       <c r="E33" s="5"/>
     </row>
     <row r="34" ht="15" customHeight="1">
@@ -2002,20 +2017,20 @@
         <v>57</v>
       </c>
       <c r="C34" t="s" s="4">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" ht="15" customHeight="1">
       <c r="A35" t="s" s="4">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s" s="4">
         <v>59</v>
       </c>
-      <c r="B35" t="s" s="4">
+      <c r="C35" t="s" s="4">
         <v>60</v>
-      </c>
-      <c r="C35" t="s" s="4">
-        <v>58</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -2028,25 +2043,23 @@
         <v>62</v>
       </c>
       <c r="C36" t="s" s="4">
-        <v>63</v>
-      </c>
-      <c r="D36" t="s" s="4">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D36" s="5"/>
       <c r="E36" s="5"/>
     </row>
     <row r="37" ht="15" customHeight="1">
       <c r="A37" t="s" s="4">
+        <v>63</v>
+      </c>
+      <c r="B37" t="s" s="4">
+        <v>64</v>
+      </c>
+      <c r="C37" t="s" s="4">
         <v>65</v>
       </c>
-      <c r="B37" t="s" s="4">
+      <c r="D37" t="s" s="4">
         <v>66</v>
-      </c>
-      <c r="C37" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="D37" t="s" s="4">
-        <v>64</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -2058,9 +2071,11 @@
         <v>68</v>
       </c>
       <c r="C38" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="D38" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="D38" t="s" s="4">
+        <v>66</v>
+      </c>
       <c r="E38" s="5"/>
     </row>
     <row r="39" ht="15" customHeight="1">
@@ -2084,141 +2099,141 @@
         <v>72</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
     </row>
     <row r="41" ht="15" customHeight="1">
       <c r="A41" t="s" s="4">
+        <v>73</v>
+      </c>
+      <c r="B41" t="s" s="4">
         <v>74</v>
       </c>
-      <c r="B41" t="s" s="4">
+      <c r="C41" t="s" s="4">
         <v>75</v>
       </c>
-      <c r="C41" t="s" s="4">
-        <v>27</v>
-      </c>
-      <c r="D41" t="s" s="4">
-        <v>64</v>
-      </c>
-      <c r="E41" t="s" s="4">
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" ht="15" customHeight="1">
+      <c r="A42" t="s" s="4">
         <v>76</v>
       </c>
-    </row>
-    <row r="42" ht="15" customHeight="1">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
+      <c r="B42" t="s" s="4">
+        <v>77</v>
+      </c>
+      <c r="C42" t="s" s="4">
+        <v>29</v>
+      </c>
+      <c r="D42" t="s" s="4">
+        <v>66</v>
+      </c>
+      <c r="E42" t="s" s="4">
+        <v>78</v>
+      </c>
     </row>
     <row r="43" ht="15" customHeight="1">
-      <c r="A43" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
     </row>
     <row r="44" ht="15" customHeight="1">
-      <c r="A44" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B44" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C44" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D44" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E44" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A44" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
     </row>
     <row r="45" ht="15" customHeight="1">
       <c r="A45" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B45" t="s" s="4">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="C45" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D45" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E45" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E45" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="46" ht="15" customHeight="1">
       <c r="A46" t="s" s="4">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="B46" t="s" s="4">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C46" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D46" t="s" s="4">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="E46" s="5"/>
     </row>
     <row r="47" ht="15" customHeight="1">
       <c r="A47" t="s" s="4">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C47" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D47" t="s" s="4">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="E47" s="5"/>
     </row>
     <row r="48" ht="15" customHeight="1">
       <c r="A48" t="s" s="4">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s" s="4">
         <v>82</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>58</v>
-      </c>
-      <c r="D48" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="D48" t="s" s="4">
+        <v>83</v>
+      </c>
       <c r="E48" s="5"/>
     </row>
     <row r="49" ht="15" customHeight="1">
       <c r="A49" t="s" s="4">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
     </row>
     <row r="50" ht="15" customHeight="1">
       <c r="A50" t="s" s="4">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="B50" t="s" s="4">
         <v>85</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
@@ -2231,99 +2246,97 @@
         <v>87</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
     </row>
     <row r="52" ht="15" customHeight="1">
       <c r="A52" t="s" s="4">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
     <row r="53" ht="15" customHeight="1">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
+      <c r="A53" t="s" s="4">
+        <v>73</v>
+      </c>
+      <c r="B53" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s" s="4">
+        <v>16</v>
+      </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
     </row>
     <row r="54" ht="15" customHeight="1">
-      <c r="A54" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
     </row>
     <row r="55" ht="15" customHeight="1">
-      <c r="A55" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B55" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C55" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D55" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E55" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A55" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
     </row>
     <row r="56" ht="15" customHeight="1">
       <c r="A56" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D56" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E56" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E56" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="57" ht="15" customHeight="1">
       <c r="A57" t="s" s="4">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C57" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D57" t="s" s="4">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="E57" s="5"/>
     </row>
     <row r="58" ht="15" customHeight="1">
       <c r="A58" t="s" s="4">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="B58" t="s" s="4">
         <v>92</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="D58" t="s" s="4">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="E58" s="5"/>
     </row>
@@ -2335,10 +2348,10 @@
         <v>94</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="D59" t="s" s="4">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="E59" s="5"/>
     </row>
@@ -2350,10 +2363,10 @@
         <v>96</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D60" t="s" s="4">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E60" s="5"/>
     </row>
@@ -2365,10 +2378,10 @@
         <v>98</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D61" t="s" s="4">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E61" s="5"/>
     </row>
@@ -2380,54 +2393,54 @@
         <v>100</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D62" t="s" s="4">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E62" s="5"/>
     </row>
     <row r="63" ht="15" customHeight="1">
       <c r="A63" t="s" s="4">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="B63" t="s" s="4">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C63" t="s" s="4">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="D63" t="s" s="4">
-        <v>64</v>
-      </c>
-      <c r="E63" t="s" s="4">
-        <v>102</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="E63" s="5"/>
     </row>
     <row r="64" ht="15" customHeight="1">
       <c r="A64" t="s" s="4">
+        <v>27</v>
+      </c>
+      <c r="B64" t="s" s="4">
         <v>103</v>
       </c>
-      <c r="B64" t="s" s="4">
+      <c r="C64" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="D64" t="s" s="4">
+        <v>66</v>
+      </c>
+      <c r="E64" t="s" s="4">
         <v>104</v>
-      </c>
-      <c r="C64" t="s" s="4">
-        <v>73</v>
-      </c>
-      <c r="D64" s="5"/>
-      <c r="E64" t="s" s="4">
-        <v>105</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1">
       <c r="A65" t="s" s="4">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="B65" t="s" s="4">
         <v>106</v>
       </c>
       <c r="C65" t="s" s="4">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" t="s" s="4">
@@ -2435,147 +2448,147 @@
       </c>
     </row>
     <row r="66" ht="15" customHeight="1">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
+      <c r="A66" t="s" s="4">
+        <v>73</v>
+      </c>
+      <c r="B66" t="s" s="4">
+        <v>108</v>
+      </c>
+      <c r="C66" t="s" s="4">
+        <v>60</v>
+      </c>
       <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
+      <c r="E66" t="s" s="4">
+        <v>109</v>
+      </c>
     </row>
     <row r="67" ht="15" customHeight="1">
-      <c r="A67" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
     </row>
     <row r="68" ht="15" customHeight="1">
-      <c r="A68" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B68" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C68" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D68" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E68" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A68" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
     </row>
     <row r="69" ht="15" customHeight="1">
       <c r="A69" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B69" t="s" s="4">
-        <v>109</v>
+        <v>2</v>
       </c>
       <c r="C69" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D69" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E69" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E69" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="70" ht="15" customHeight="1">
       <c r="A70" t="s" s="4">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="B70" t="s" s="4">
         <v>111</v>
       </c>
       <c r="C70" t="s" s="4">
-        <v>16</v>
-      </c>
-      <c r="D70" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="D70" t="s" s="4">
+        <v>9</v>
+      </c>
       <c r="E70" s="5"/>
     </row>
     <row r="71" ht="15" customHeight="1">
       <c r="A71" t="s" s="4">
-        <v>61</v>
+        <v>112</v>
       </c>
       <c r="B71" t="s" s="4">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C71" t="s" s="4">
-        <v>63</v>
-      </c>
-      <c r="D71" t="s" s="4">
-        <v>64</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D71" s="5"/>
       <c r="E71" s="5"/>
     </row>
     <row r="72" ht="15" customHeight="1">
       <c r="A72" t="s" s="4">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="B72" t="s" s="4">
         <v>114</v>
       </c>
       <c r="C72" t="s" s="4">
+        <v>65</v>
+      </c>
+      <c r="D72" t="s" s="4">
+        <v>66</v>
+      </c>
+      <c r="E72" s="5"/>
+    </row>
+    <row r="73" ht="15" customHeight="1">
+      <c r="A73" t="s" s="4">
+        <v>115</v>
+      </c>
+      <c r="B73" t="s" s="4">
+        <v>116</v>
+      </c>
+      <c r="C73" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="D72" t="s" s="4">
-        <v>115</v>
-      </c>
-      <c r="E72" s="5"/>
-    </row>
-    <row r="73" ht="15" customHeight="1">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
+      <c r="D73" t="s" s="4">
+        <v>117</v>
+      </c>
       <c r="E73" s="5"/>
     </row>
     <row r="74" ht="15" customHeight="1">
-      <c r="A74" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
     </row>
     <row r="75" ht="15" customHeight="1">
-      <c r="A75" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B75" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C75" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D75" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E75" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A75" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
     </row>
     <row r="76" ht="15" customHeight="1">
       <c r="A76" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B76" t="s" s="4">
-        <v>117</v>
+        <v>2</v>
       </c>
       <c r="C76" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D76" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E76" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E76" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="77" ht="15" customHeight="1">
       <c r="A77" t="s" s="4">
-        <v>118</v>
+        <v>6</v>
       </c>
       <c r="B77" t="s" s="4">
         <v>119</v>
@@ -2584,78 +2597,93 @@
         <v>8</v>
       </c>
       <c r="D77" t="s" s="4">
-        <v>120</v>
+        <v>9</v>
       </c>
       <c r="E77" s="5"/>
     </row>
     <row r="78" ht="15" customHeight="1">
       <c r="A78" t="s" s="4">
+        <v>120</v>
+      </c>
+      <c r="B78" t="s" s="4">
         <v>121</v>
-      </c>
-      <c r="B78" t="s" s="4">
-        <v>122</v>
       </c>
       <c r="C78" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D78" t="s" s="4">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E78" s="5"/>
     </row>
     <row r="79" ht="15" customHeight="1">
       <c r="A79" t="s" s="4">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="B79" t="s" s="4">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C79" t="s" s="4">
-        <v>124</v>
+        <v>8</v>
       </c>
       <c r="D79" t="s" s="4">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E79" s="5"/>
     </row>
     <row r="80" ht="15" customHeight="1">
       <c r="A80" t="s" s="4">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="B80" t="s" s="4">
-        <v>5</v>
+        <v>125</v>
       </c>
       <c r="C80" t="s" s="4">
-        <v>125</v>
-      </c>
-      <c r="D80" s="5"/>
+        <v>126</v>
+      </c>
+      <c r="D80" t="s" s="4">
+        <v>117</v>
+      </c>
       <c r="E80" s="5"/>
     </row>
     <row r="81" ht="15" customHeight="1">
       <c r="A81" t="s" s="4">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="B81" t="s" s="4">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="C81" t="s" s="4">
+        <v>127</v>
+      </c>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+    </row>
+    <row r="82" ht="15" customHeight="1">
+      <c r="A82" t="s" s="4">
+        <v>37</v>
+      </c>
+      <c r="B82" t="s" s="4">
+        <v>128</v>
+      </c>
+      <c r="C82" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="D81" t="s" s="4">
-        <v>127</v>
-      </c>
-      <c r="E81" s="5"/>
+      <c r="D82" t="s" s="4">
+        <v>129</v>
+      </c>
+      <c r="E82" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A74:E74"/>
-    <mergeCell ref="A54:E54"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A67:E67"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A75:E75"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511806" footer="0.511806"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
change position to position_x and position_y
</commit_message>
<xml_diff>
--- a/数据库/db.xlsx
+++ b/数据库/db.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="132">
   <si>
     <t>用户表-user</t>
   </si>
@@ -118,10 +118,19 @@
     <t>primary key not null</t>
   </si>
   <si>
-    <t>position</t>
-  </si>
-  <si>
-    <t>即时位置</t>
+    <t>position_x</t>
+  </si>
+  <si>
+    <t>即时位置 x</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>position_y</t>
+  </si>
+  <si>
+    <t>即时位置 y</t>
   </si>
   <si>
     <t>score</t>
@@ -206,9 +215,6 @@
   </si>
   <si>
     <t>费用</t>
-  </si>
-  <si>
-    <t>double</t>
   </si>
   <si>
     <t>default 0</t>
@@ -1570,7 +1576,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1771,20 +1777,22 @@
         <v>36</v>
       </c>
       <c r="C14" t="s" s="4">
-        <v>16</v>
-      </c>
-      <c r="D14" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="D14" t="s" s="4">
+        <v>30</v>
+      </c>
       <c r="E14" s="5"/>
     </row>
     <row r="15" ht="15" customHeight="1">
       <c r="A15" t="s" s="4">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s" s="4">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s" s="4">
         <v>37</v>
-      </c>
-      <c r="B15" t="s" s="4">
-        <v>38</v>
-      </c>
-      <c r="C15" t="s" s="4">
-        <v>8</v>
       </c>
       <c r="D15" t="s" s="4">
         <v>30</v>
@@ -1792,75 +1800,77 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" ht="15" customHeight="1">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="A16" t="s" s="4">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s" s="4">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s" s="4">
+        <v>30</v>
+      </c>
       <c r="E16" s="5"/>
     </row>
     <row r="17" ht="15" customHeight="1">
-      <c r="A17" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" ht="15" customHeight="1">
-      <c r="A18" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D18" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E18" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A18" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" ht="15" customHeight="1">
       <c r="A19" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D19" t="s" s="4">
-        <v>34</v>
-      </c>
-      <c r="E19" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E19" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" ht="15" customHeight="1">
       <c r="A20" t="s" s="4">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s" s="4">
-        <v>16</v>
-      </c>
-      <c r="D20" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="D20" t="s" s="4">
+        <v>34</v>
+      </c>
       <c r="E20" s="5"/>
     </row>
     <row r="21" ht="15" customHeight="1">
       <c r="A21" t="s" s="4">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s" s="4">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s" s="4">
         <v>37</v>
-      </c>
-      <c r="B21" t="s" s="4">
-        <v>40</v>
-      </c>
-      <c r="C21" t="s" s="4">
-        <v>8</v>
       </c>
       <c r="D21" t="s" s="4">
         <v>30</v>
@@ -1869,47 +1879,63 @@
     </row>
     <row r="22" ht="15" customHeight="1">
       <c r="A22" t="s" s="4">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s" s="4">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s" s="4">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E22" s="5"/>
     </row>
     <row r="23" ht="15" customHeight="1">
       <c r="A23" t="s" s="4">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s" s="4">
         <v>43</v>
       </c>
-      <c r="B23" t="s" s="4">
+      <c r="C23" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s" s="4">
+        <v>30</v>
+      </c>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" ht="15" customHeight="1">
+      <c r="A24" t="s" s="4">
         <v>44</v>
       </c>
-      <c r="C23" t="s" s="4">
+      <c r="B24" t="s" s="4">
         <v>45</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" ht="15" customHeight="1">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+      <c r="C24" t="s" s="4">
+        <v>16</v>
+      </c>
+      <c r="D24" t="s" s="4">
+        <v>13</v>
+      </c>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" ht="12.75" customHeight="1" hidden="1">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+    <row r="25" ht="15" customHeight="1">
+      <c r="A25" t="s" s="4">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s" s="4">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s" s="4">
+        <v>48</v>
+      </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" ht="12.75" customHeight="1" hidden="1">
+    <row r="26" ht="15" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1923,283 +1949,267 @@
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" ht="15" customHeight="1">
-      <c r="A28" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" ht="15" customHeight="1">
-      <c r="A29" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D29" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E29" t="s" s="4">
-        <v>5</v>
-      </c>
+    <row r="28" ht="12.75" customHeight="1" hidden="1">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" ht="12.75" customHeight="1" hidden="1">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
     </row>
     <row r="30" ht="15" customHeight="1">
-      <c r="A30" t="s" s="4">
-        <v>6</v>
-      </c>
-      <c r="B30" t="s" s="4">
-        <v>47</v>
-      </c>
-      <c r="C30" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="D30" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E30" s="5"/>
+      <c r="A30" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
     </row>
     <row r="31" ht="15" customHeight="1">
       <c r="A31" t="s" s="4">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D31" t="s" s="4">
-        <v>50</v>
-      </c>
-      <c r="E31" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E31" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" ht="15" customHeight="1">
       <c r="A32" t="s" s="4">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D32" t="s" s="4">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="E32" s="5"/>
     </row>
     <row r="33" ht="15" customHeight="1">
       <c r="A33" t="s" s="4">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s" s="4">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D33" t="s" s="4">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="E33" s="5"/>
     </row>
     <row r="34" ht="15" customHeight="1">
       <c r="A34" t="s" s="4">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s" s="4">
+        <v>55</v>
+      </c>
+      <c r="C34" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s" s="4">
         <v>56</v>
       </c>
-      <c r="B34" t="s" s="4">
-        <v>57</v>
-      </c>
-      <c r="C34" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" ht="15" customHeight="1">
       <c r="A35" t="s" s="4">
+        <v>57</v>
+      </c>
+      <c r="B35" t="s" s="4">
         <v>58</v>
       </c>
-      <c r="B35" t="s" s="4">
-        <v>59</v>
-      </c>
       <c r="C35" t="s" s="4">
-        <v>60</v>
-      </c>
-      <c r="D35" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="D35" t="s" s="4">
+        <v>21</v>
+      </c>
       <c r="E35" s="5"/>
     </row>
     <row r="36" ht="15" customHeight="1">
       <c r="A36" t="s" s="4">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C36" t="s" s="4">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
     </row>
     <row r="37" ht="15" customHeight="1">
       <c r="A37" t="s" s="4">
+        <v>61</v>
+      </c>
+      <c r="B37" t="s" s="4">
+        <v>62</v>
+      </c>
+      <c r="C37" t="s" s="4">
         <v>63</v>
       </c>
-      <c r="B37" t="s" s="4">
-        <v>64</v>
-      </c>
-      <c r="C37" t="s" s="4">
-        <v>65</v>
-      </c>
-      <c r="D37" t="s" s="4">
-        <v>66</v>
-      </c>
+      <c r="D37" s="5"/>
       <c r="E37" s="5"/>
     </row>
     <row r="38" ht="15" customHeight="1">
       <c r="A38" t="s" s="4">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="D38" t="s" s="4">
-        <v>66</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D38" s="5"/>
       <c r="E38" s="5"/>
     </row>
     <row r="39" ht="15" customHeight="1">
       <c r="A39" t="s" s="4">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B39" t="s" s="4">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C39" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="D39" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="D39" t="s" s="4">
+        <v>68</v>
+      </c>
       <c r="E39" s="5"/>
     </row>
     <row r="40" ht="15" customHeight="1">
       <c r="A40" t="s" s="4">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="D40" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="D40" t="s" s="4">
+        <v>68</v>
+      </c>
       <c r="E40" s="5"/>
     </row>
     <row r="41" ht="15" customHeight="1">
       <c r="A41" t="s" s="4">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s" s="4">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" ht="15" customHeight="1">
       <c r="A42" t="s" s="4">
+        <v>73</v>
+      </c>
+      <c r="B42" t="s" s="4">
+        <v>74</v>
+      </c>
+      <c r="C42" t="s" s="4">
+        <v>20</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" ht="15" customHeight="1">
+      <c r="A43" t="s" s="4">
+        <v>75</v>
+      </c>
+      <c r="B43" t="s" s="4">
         <v>76</v>
       </c>
-      <c r="B42" t="s" s="4">
+      <c r="C43" t="s" s="4">
         <v>77</v>
       </c>
-      <c r="C42" t="s" s="4">
-        <v>29</v>
-      </c>
-      <c r="D42" t="s" s="4">
-        <v>66</v>
-      </c>
-      <c r="E42" t="s" s="4">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="43" ht="15" customHeight="1">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
     <row r="44" ht="15" customHeight="1">
-      <c r="A44" t="s" s="2">
+      <c r="A44" t="s" s="4">
+        <v>78</v>
+      </c>
+      <c r="B44" t="s" s="4">
         <v>79</v>
       </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
+      <c r="C44" t="s" s="4">
+        <v>29</v>
+      </c>
+      <c r="D44" t="s" s="4">
+        <v>68</v>
+      </c>
+      <c r="E44" t="s" s="4">
+        <v>80</v>
+      </c>
     </row>
     <row r="45" ht="15" customHeight="1">
-      <c r="A45" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C45" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D45" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E45" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
     </row>
     <row r="46" ht="15" customHeight="1">
-      <c r="A46" t="s" s="4">
-        <v>6</v>
-      </c>
-      <c r="B46" t="s" s="4">
-        <v>80</v>
-      </c>
-      <c r="C46" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="D46" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E46" s="5"/>
+      <c r="A46" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
     </row>
     <row r="47" ht="15" customHeight="1">
       <c r="A47" t="s" s="4">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>81</v>
+        <v>2</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D47" t="s" s="4">
-        <v>50</v>
-      </c>
-      <c r="E47" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E47" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="48" ht="15" customHeight="1">
       <c r="A48" t="s" s="4">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B48" t="s" s="4">
         <v>82</v>
@@ -2208,482 +2218,512 @@
         <v>8</v>
       </c>
       <c r="D48" t="s" s="4">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="E48" s="5"/>
     </row>
     <row r="49" ht="15" customHeight="1">
       <c r="A49" t="s" s="4">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>60</v>
-      </c>
-      <c r="D49" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="D49" t="s" s="4">
+        <v>53</v>
+      </c>
       <c r="E49" s="5"/>
     </row>
     <row r="50" ht="15" customHeight="1">
       <c r="A50" t="s" s="4">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B50" t="s" s="4">
+        <v>84</v>
+      </c>
+      <c r="C50" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s" s="4">
         <v>85</v>
       </c>
-      <c r="C50" t="s" s="4">
-        <v>60</v>
-      </c>
-      <c r="D50" s="5"/>
       <c r="E50" s="5"/>
     </row>
     <row r="51" ht="15" customHeight="1">
       <c r="A51" t="s" s="4">
+        <v>61</v>
+      </c>
+      <c r="B51" t="s" s="4">
         <v>86</v>
       </c>
-      <c r="B51" t="s" s="4">
-        <v>87</v>
-      </c>
       <c r="C51" t="s" s="4">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
     </row>
     <row r="52" ht="15" customHeight="1">
       <c r="A52" t="s" s="4">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
     <row r="53" ht="15" customHeight="1">
       <c r="A53" t="s" s="4">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
     </row>
     <row r="54" ht="15" customHeight="1">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
+      <c r="A54" t="s" s="4">
+        <v>90</v>
+      </c>
+      <c r="B54" t="s" s="4">
+        <v>91</v>
+      </c>
+      <c r="C54" t="s" s="4">
+        <v>20</v>
+      </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
     </row>
     <row r="55" ht="15" customHeight="1">
-      <c r="A55" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
+      <c r="A55" t="s" s="4">
+        <v>75</v>
+      </c>
+      <c r="B55" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s" s="4">
+        <v>16</v>
+      </c>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
     </row>
     <row r="56" ht="15" customHeight="1">
-      <c r="A56" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B56" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C56" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D56" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E56" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
     </row>
     <row r="57" ht="15" customHeight="1">
-      <c r="A57" t="s" s="4">
-        <v>6</v>
-      </c>
-      <c r="B57" t="s" s="4">
-        <v>91</v>
-      </c>
-      <c r="C57" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="D57" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E57" s="5"/>
+      <c r="A57" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
     </row>
     <row r="58" ht="15" customHeight="1">
       <c r="A58" t="s" s="4">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>92</v>
+        <v>2</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D58" t="s" s="4">
-        <v>50</v>
-      </c>
-      <c r="E58" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E58" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="59" ht="15" customHeight="1">
       <c r="A59" t="s" s="4">
+        <v>6</v>
+      </c>
+      <c r="B59" t="s" s="4">
         <v>93</v>
       </c>
-      <c r="B59" t="s" s="4">
-        <v>94</v>
-      </c>
       <c r="C59" t="s" s="4">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="D59" t="s" s="4">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E59" s="5"/>
     </row>
     <row r="60" ht="15" customHeight="1">
       <c r="A60" t="s" s="4">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="D60" t="s" s="4">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="E60" s="5"/>
     </row>
     <row r="61" ht="15" customHeight="1">
       <c r="A61" t="s" s="4">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D61" t="s" s="4">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="E61" s="5"/>
     </row>
     <row r="62" ht="15" customHeight="1">
       <c r="A62" t="s" s="4">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="D62" t="s" s="4">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E62" s="5"/>
     </row>
     <row r="63" ht="15" customHeight="1">
       <c r="A63" t="s" s="4">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B63" t="s" s="4">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C63" t="s" s="4">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="D63" t="s" s="4">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E63" s="5"/>
     </row>
     <row r="64" ht="15" customHeight="1">
       <c r="A64" t="s" s="4">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="B64" t="s" s="4">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C64" t="s" s="4">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="D64" t="s" s="4">
-        <v>66</v>
-      </c>
-      <c r="E64" t="s" s="4">
-        <v>104</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="E64" s="5"/>
     </row>
     <row r="65" ht="15" customHeight="1">
       <c r="A65" t="s" s="4">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B65" t="s" s="4">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C65" t="s" s="4">
-        <v>75</v>
-      </c>
-      <c r="D65" s="5"/>
-      <c r="E65" t="s" s="4">
-        <v>107</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D65" t="s" s="4">
+        <v>68</v>
+      </c>
+      <c r="E65" s="5"/>
     </row>
     <row r="66" ht="15" customHeight="1">
       <c r="A66" t="s" s="4">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="B66" t="s" s="4">
+        <v>105</v>
+      </c>
+      <c r="C66" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="D66" t="s" s="4">
+        <v>68</v>
+      </c>
+      <c r="E66" t="s" s="4">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="67" ht="15" customHeight="1">
+      <c r="A67" t="s" s="4">
+        <v>107</v>
+      </c>
+      <c r="B67" t="s" s="4">
         <v>108</v>
       </c>
-      <c r="C66" t="s" s="4">
-        <v>60</v>
-      </c>
-      <c r="D66" s="5"/>
-      <c r="E66" t="s" s="4">
+      <c r="C67" t="s" s="4">
+        <v>77</v>
+      </c>
+      <c r="D67" s="5"/>
+      <c r="E67" t="s" s="4">
         <v>109</v>
       </c>
     </row>
-    <row r="67" ht="15" customHeight="1">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-    </row>
     <row r="68" ht="15" customHeight="1">
-      <c r="A68" t="s" s="2">
+      <c r="A68" t="s" s="4">
+        <v>75</v>
+      </c>
+      <c r="B68" t="s" s="4">
         <v>110</v>
       </c>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
+      <c r="C68" t="s" s="4">
+        <v>63</v>
+      </c>
+      <c r="D68" s="5"/>
+      <c r="E68" t="s" s="4">
+        <v>111</v>
+      </c>
     </row>
     <row r="69" ht="15" customHeight="1">
-      <c r="A69" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B69" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C69" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D69" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E69" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
     </row>
     <row r="70" ht="15" customHeight="1">
-      <c r="A70" t="s" s="4">
-        <v>6</v>
-      </c>
-      <c r="B70" t="s" s="4">
-        <v>111</v>
-      </c>
-      <c r="C70" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="D70" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E70" s="5"/>
+      <c r="A70" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
     </row>
     <row r="71" ht="15" customHeight="1">
       <c r="A71" t="s" s="4">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="B71" t="s" s="4">
-        <v>113</v>
+        <v>2</v>
       </c>
       <c r="C71" t="s" s="4">
-        <v>16</v>
-      </c>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="D71" t="s" s="4">
+        <v>4</v>
+      </c>
+      <c r="E71" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="72" ht="15" customHeight="1">
       <c r="A72" t="s" s="4">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="B72" t="s" s="4">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C72" t="s" s="4">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="D72" t="s" s="4">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="E72" s="5"/>
     </row>
     <row r="73" ht="15" customHeight="1">
       <c r="A73" t="s" s="4">
+        <v>114</v>
+      </c>
+      <c r="B73" t="s" s="4">
         <v>115</v>
       </c>
-      <c r="B73" t="s" s="4">
+      <c r="C73" t="s" s="4">
+        <v>16</v>
+      </c>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+    </row>
+    <row r="74" ht="15" customHeight="1">
+      <c r="A74" t="s" s="4">
+        <v>66</v>
+      </c>
+      <c r="B74" t="s" s="4">
         <v>116</v>
       </c>
-      <c r="C73" t="s" s="4">
+      <c r="C74" t="s" s="4">
+        <v>37</v>
+      </c>
+      <c r="D74" t="s" s="4">
+        <v>68</v>
+      </c>
+      <c r="E74" s="5"/>
+    </row>
+    <row r="75" ht="15" customHeight="1">
+      <c r="A75" t="s" s="4">
+        <v>117</v>
+      </c>
+      <c r="B75" t="s" s="4">
+        <v>118</v>
+      </c>
+      <c r="C75" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="D73" t="s" s="4">
-        <v>117</v>
-      </c>
-      <c r="E73" s="5"/>
-    </row>
-    <row r="74" ht="15" customHeight="1">
-      <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-    </row>
-    <row r="75" ht="15" customHeight="1">
-      <c r="A75" t="s" s="2">
-        <v>118</v>
-      </c>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
+      <c r="D75" t="s" s="4">
+        <v>119</v>
+      </c>
+      <c r="E75" s="5"/>
     </row>
     <row r="76" ht="15" customHeight="1">
-      <c r="A76" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B76" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C76" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D76" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E76" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
     </row>
     <row r="77" ht="15" customHeight="1">
-      <c r="A77" t="s" s="4">
-        <v>6</v>
-      </c>
-      <c r="B77" t="s" s="4">
-        <v>119</v>
-      </c>
-      <c r="C77" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="D77" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E77" s="5"/>
+      <c r="A77" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
     </row>
     <row r="78" ht="15" customHeight="1">
       <c r="A78" t="s" s="4">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="B78" t="s" s="4">
-        <v>121</v>
+        <v>2</v>
       </c>
       <c r="C78" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D78" t="s" s="4">
-        <v>122</v>
-      </c>
-      <c r="E78" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E78" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="79" ht="15" customHeight="1">
       <c r="A79" t="s" s="4">
-        <v>123</v>
+        <v>6</v>
       </c>
       <c r="B79" t="s" s="4">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C79" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D79" t="s" s="4">
-        <v>122</v>
+        <v>9</v>
       </c>
       <c r="E79" s="5"/>
     </row>
     <row r="80" ht="15" customHeight="1">
       <c r="A80" t="s" s="4">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B80" t="s" s="4">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C80" t="s" s="4">
-        <v>126</v>
+        <v>8</v>
       </c>
       <c r="D80" t="s" s="4">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="E80" s="5"/>
     </row>
     <row r="81" ht="15" customHeight="1">
       <c r="A81" t="s" s="4">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="B81" t="s" s="4">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="C81" t="s" s="4">
-        <v>127</v>
-      </c>
-      <c r="D81" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="D81" t="s" s="4">
+        <v>124</v>
+      </c>
       <c r="E81" s="5"/>
     </row>
     <row r="82" ht="15" customHeight="1">
       <c r="A82" t="s" s="4">
-        <v>37</v>
+        <v>117</v>
       </c>
       <c r="B82" t="s" s="4">
+        <v>127</v>
+      </c>
+      <c r="C82" t="s" s="4">
         <v>128</v>
       </c>
-      <c r="C82" t="s" s="4">
+      <c r="D82" t="s" s="4">
+        <v>119</v>
+      </c>
+      <c r="E82" s="5"/>
+    </row>
+    <row r="83" ht="15" customHeight="1">
+      <c r="A83" t="s" s="4">
+        <v>75</v>
+      </c>
+      <c r="B83" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="C83" t="s" s="4">
+        <v>129</v>
+      </c>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+    </row>
+    <row r="84" ht="15" customHeight="1">
+      <c r="A84" t="s" s="4">
+        <v>40</v>
+      </c>
+      <c r="B84" t="s" s="4">
+        <v>130</v>
+      </c>
+      <c r="C84" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="D82" t="s" s="4">
-        <v>129</v>
-      </c>
-      <c r="E82" s="5"/>
+      <c r="D84" t="s" s="4">
+        <v>131</v>
+      </c>
+      <c r="E84" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A77:E77"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A70:E70"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A46:E46"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A75:E75"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511806" footer="0.511806"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
add password for lessee
</commit_message>
<xml_diff>
--- a/数据库/db.xlsx
+++ b/数据库/db.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="134">
   <si>
     <t>用户表-user</t>
   </si>
@@ -142,6 +142,15 @@
     <t>用户(货车司机)扩展表-lessee</t>
   </si>
   <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>用户密码</t>
+  </si>
+  <si>
+    <t>varchar(256)</t>
+  </si>
+  <si>
     <t>用户信誉积分</t>
   </si>
   <si>
@@ -242,9 +251,6 @@
   </si>
   <si>
     <t>租车人对订单的评价</t>
-  </si>
-  <si>
-    <t>varchar(256)</t>
   </si>
   <si>
     <t>status</t>
@@ -1576,7 +1582,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1864,25 +1870,23 @@
     </row>
     <row r="21" ht="15" customHeight="1">
       <c r="A21" t="s" s="4">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s" s="4">
-        <v>37</v>
-      </c>
-      <c r="D21" t="s" s="4">
-        <v>30</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D21" s="4"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" ht="15" customHeight="1">
       <c r="A22" t="s" s="4">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s" s="4">
         <v>37</v>
@@ -1894,13 +1898,13 @@
     </row>
     <row r="23" ht="15" customHeight="1">
       <c r="A23" t="s" s="4">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s" s="4">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s" s="4">
         <v>30</v>
@@ -1909,40 +1913,48 @@
     </row>
     <row r="24" ht="15" customHeight="1">
       <c r="A24" t="s" s="4">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s" s="4">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D24" t="s" s="4">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E24" s="5"/>
     </row>
     <row r="25" ht="15" customHeight="1">
       <c r="A25" t="s" s="4">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s" s="4">
-        <v>48</v>
-      </c>
-      <c r="D25" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="D25" t="s" s="4">
+        <v>13</v>
+      </c>
       <c r="E25" s="5"/>
     </row>
     <row r="26" ht="15" customHeight="1">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="A26" t="s" s="4">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s" s="4">
+        <v>50</v>
+      </c>
+      <c r="C26" t="s" s="4">
+        <v>51</v>
+      </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" ht="12.75" customHeight="1" hidden="1">
+    <row r="27" ht="15" customHeight="1">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1963,59 +1975,51 @@
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" ht="15" customHeight="1">
-      <c r="A30" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+    <row r="30" ht="12.75" customHeight="1" hidden="1">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" ht="15" customHeight="1">
-      <c r="A31" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D31" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E31" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A31" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
     </row>
     <row r="32" ht="15" customHeight="1">
       <c r="A32" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D32" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E32" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E32" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" ht="15" customHeight="1">
       <c r="A33" t="s" s="4">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D33" t="s" s="4">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -2042,35 +2046,37 @@
         <v>58</v>
       </c>
       <c r="C35" t="s" s="4">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D35" t="s" s="4">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="E35" s="5"/>
     </row>
     <row r="36" ht="15" customHeight="1">
       <c r="A36" t="s" s="4">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="D36" s="5"/>
+      <c r="D36" t="s" s="4">
+        <v>21</v>
+      </c>
       <c r="E36" s="5"/>
     </row>
     <row r="37" ht="15" customHeight="1">
       <c r="A37" t="s" s="4">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C37" t="s" s="4">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -2083,24 +2089,22 @@
         <v>65</v>
       </c>
       <c r="C38" t="s" s="4">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
     </row>
     <row r="39" ht="15" customHeight="1">
       <c r="A39" t="s" s="4">
+        <v>67</v>
+      </c>
+      <c r="B39" t="s" s="4">
+        <v>68</v>
+      </c>
+      <c r="C39" t="s" s="4">
         <v>66</v>
       </c>
-      <c r="B39" t="s" s="4">
-        <v>67</v>
-      </c>
-      <c r="C39" t="s" s="4">
-        <v>37</v>
-      </c>
-      <c r="D39" t="s" s="4">
-        <v>68</v>
-      </c>
+      <c r="D39" s="5"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" ht="15" customHeight="1">
@@ -2111,32 +2115,34 @@
         <v>70</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="D40" t="s" s="4">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E40" s="5"/>
     </row>
     <row r="41" ht="15" customHeight="1">
       <c r="A41" t="s" s="4">
+        <v>72</v>
+      </c>
+      <c r="B41" t="s" s="4">
+        <v>73</v>
+      </c>
+      <c r="C41" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s" s="4">
         <v>71</v>
       </c>
-      <c r="B41" t="s" s="4">
-        <v>72</v>
-      </c>
-      <c r="C41" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="D41" s="5"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" ht="15" customHeight="1">
       <c r="A42" t="s" s="4">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s" s="4">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s" s="4">
         <v>20</v>
@@ -2146,13 +2152,13 @@
     </row>
     <row r="43" ht="15" customHeight="1">
       <c r="A43" t="s" s="4">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -2165,75 +2171,73 @@
         <v>79</v>
       </c>
       <c r="C44" t="s" s="4">
+        <v>45</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" ht="15" customHeight="1">
+      <c r="A45" t="s" s="4">
+        <v>80</v>
+      </c>
+      <c r="B45" t="s" s="4">
+        <v>81</v>
+      </c>
+      <c r="C45" t="s" s="4">
         <v>29</v>
       </c>
-      <c r="D44" t="s" s="4">
-        <v>68</v>
-      </c>
-      <c r="E44" t="s" s="4">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="45" ht="15" customHeight="1">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
+      <c r="D45" t="s" s="4">
+        <v>71</v>
+      </c>
+      <c r="E45" t="s" s="4">
+        <v>82</v>
+      </c>
     </row>
     <row r="46" ht="15" customHeight="1">
-      <c r="A46" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
     </row>
     <row r="47" ht="15" customHeight="1">
-      <c r="A47" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C47" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D47" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E47" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A47" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
     </row>
     <row r="48" ht="15" customHeight="1">
       <c r="A48" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B48" t="s" s="4">
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D48" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E48" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E48" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="49" ht="15" customHeight="1">
       <c r="A49" t="s" s="4">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C49" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D49" t="s" s="4">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -2242,27 +2246,29 @@
         <v>54</v>
       </c>
       <c r="B50" t="s" s="4">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C50" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D50" t="s" s="4">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="E50" s="5"/>
     </row>
     <row r="51" ht="15" customHeight="1">
       <c r="A51" t="s" s="4">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B51" t="s" s="4">
         <v>86</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>63</v>
-      </c>
-      <c r="D51" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="D51" t="s" s="4">
+        <v>87</v>
+      </c>
       <c r="E51" s="5"/>
     </row>
     <row r="52" ht="15" customHeight="1">
@@ -2270,23 +2276,23 @@
         <v>64</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
     <row r="53" ht="15" customHeight="1">
       <c r="A53" t="s" s="4">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="B53" t="s" s="4">
         <v>89</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
@@ -2299,99 +2305,97 @@
         <v>91</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
     </row>
     <row r="55" ht="15" customHeight="1">
       <c r="A55" t="s" s="4">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
     </row>
     <row r="56" ht="15" customHeight="1">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
+      <c r="A56" t="s" s="4">
+        <v>78</v>
+      </c>
+      <c r="B56" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s" s="4">
+        <v>16</v>
+      </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
     </row>
     <row r="57" ht="15" customHeight="1">
-      <c r="A57" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
     </row>
     <row r="58" ht="15" customHeight="1">
-      <c r="A58" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B58" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C58" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D58" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E58" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A58" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
     </row>
     <row r="59" ht="15" customHeight="1">
       <c r="A59" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D59" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E59" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E59" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="60" ht="15" customHeight="1">
       <c r="A60" t="s" s="4">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C60" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D60" t="s" s="4">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="E60" s="5"/>
     </row>
     <row r="61" ht="15" customHeight="1">
       <c r="A61" t="s" s="4">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="B61" t="s" s="4">
         <v>96</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="D61" t="s" s="4">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="E61" s="5"/>
     </row>
@@ -2403,10 +2407,10 @@
         <v>98</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="D62" t="s" s="4">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="E62" s="5"/>
     </row>
@@ -2421,7 +2425,7 @@
         <v>37</v>
       </c>
       <c r="D63" t="s" s="4">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E63" s="5"/>
     </row>
@@ -2436,7 +2440,7 @@
         <v>37</v>
       </c>
       <c r="D64" t="s" s="4">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E64" s="5"/>
     </row>
@@ -2451,51 +2455,51 @@
         <v>37</v>
       </c>
       <c r="D65" t="s" s="4">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E65" s="5"/>
     </row>
     <row r="66" ht="15" customHeight="1">
       <c r="A66" t="s" s="4">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="B66" t="s" s="4">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C66" t="s" s="4">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="D66" t="s" s="4">
-        <v>68</v>
-      </c>
-      <c r="E66" t="s" s="4">
-        <v>106</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="E66" s="5"/>
     </row>
     <row r="67" ht="15" customHeight="1">
       <c r="A67" t="s" s="4">
+        <v>27</v>
+      </c>
+      <c r="B67" t="s" s="4">
         <v>107</v>
       </c>
-      <c r="B67" t="s" s="4">
+      <c r="C67" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="D67" t="s" s="4">
+        <v>71</v>
+      </c>
+      <c r="E67" t="s" s="4">
         <v>108</v>
-      </c>
-      <c r="C67" t="s" s="4">
-        <v>77</v>
-      </c>
-      <c r="D67" s="5"/>
-      <c r="E67" t="s" s="4">
-        <v>109</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1">
       <c r="A68" t="s" s="4">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="B68" t="s" s="4">
         <v>110</v>
       </c>
       <c r="C68" t="s" s="4">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" t="s" s="4">
@@ -2503,147 +2507,147 @@
       </c>
     </row>
     <row r="69" ht="15" customHeight="1">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
+      <c r="A69" t="s" s="4">
+        <v>78</v>
+      </c>
+      <c r="B69" t="s" s="4">
+        <v>112</v>
+      </c>
+      <c r="C69" t="s" s="4">
+        <v>66</v>
+      </c>
       <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
+      <c r="E69" t="s" s="4">
+        <v>113</v>
+      </c>
     </row>
     <row r="70" ht="15" customHeight="1">
-      <c r="A70" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
     </row>
     <row r="71" ht="15" customHeight="1">
-      <c r="A71" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B71" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C71" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D71" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E71" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A71" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
     </row>
     <row r="72" ht="15" customHeight="1">
       <c r="A72" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B72" t="s" s="4">
-        <v>113</v>
+        <v>2</v>
       </c>
       <c r="C72" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D72" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E72" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E72" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="73" ht="15" customHeight="1">
       <c r="A73" t="s" s="4">
-        <v>114</v>
+        <v>6</v>
       </c>
       <c r="B73" t="s" s="4">
         <v>115</v>
       </c>
       <c r="C73" t="s" s="4">
-        <v>16</v>
-      </c>
-      <c r="D73" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="D73" t="s" s="4">
+        <v>9</v>
+      </c>
       <c r="E73" s="5"/>
     </row>
     <row r="74" ht="15" customHeight="1">
       <c r="A74" t="s" s="4">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="B74" t="s" s="4">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C74" t="s" s="4">
-        <v>37</v>
-      </c>
-      <c r="D74" t="s" s="4">
-        <v>68</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D74" s="5"/>
       <c r="E74" s="5"/>
     </row>
     <row r="75" ht="15" customHeight="1">
       <c r="A75" t="s" s="4">
-        <v>117</v>
+        <v>69</v>
       </c>
       <c r="B75" t="s" s="4">
         <v>118</v>
       </c>
       <c r="C75" t="s" s="4">
+        <v>37</v>
+      </c>
+      <c r="D75" t="s" s="4">
+        <v>71</v>
+      </c>
+      <c r="E75" s="5"/>
+    </row>
+    <row r="76" ht="15" customHeight="1">
+      <c r="A76" t="s" s="4">
+        <v>119</v>
+      </c>
+      <c r="B76" t="s" s="4">
+        <v>120</v>
+      </c>
+      <c r="C76" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="D75" t="s" s="4">
-        <v>119</v>
-      </c>
-      <c r="E75" s="5"/>
-    </row>
-    <row r="76" ht="15" customHeight="1">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
+      <c r="D76" t="s" s="4">
+        <v>121</v>
+      </c>
       <c r="E76" s="5"/>
     </row>
     <row r="77" ht="15" customHeight="1">
-      <c r="A77" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
     </row>
     <row r="78" ht="15" customHeight="1">
-      <c r="A78" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B78" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C78" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D78" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E78" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A78" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
     </row>
     <row r="79" ht="15" customHeight="1">
       <c r="A79" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B79" t="s" s="4">
-        <v>121</v>
+        <v>2</v>
       </c>
       <c r="C79" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D79" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E79" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E79" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="80" ht="15" customHeight="1">
       <c r="A80" t="s" s="4">
-        <v>122</v>
+        <v>6</v>
       </c>
       <c r="B80" t="s" s="4">
         <v>123</v>
@@ -2652,78 +2656,93 @@
         <v>8</v>
       </c>
       <c r="D80" t="s" s="4">
-        <v>124</v>
+        <v>9</v>
       </c>
       <c r="E80" s="5"/>
     </row>
     <row r="81" ht="15" customHeight="1">
       <c r="A81" t="s" s="4">
+        <v>124</v>
+      </c>
+      <c r="B81" t="s" s="4">
         <v>125</v>
-      </c>
-      <c r="B81" t="s" s="4">
-        <v>126</v>
       </c>
       <c r="C81" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D81" t="s" s="4">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E81" s="5"/>
     </row>
     <row r="82" ht="15" customHeight="1">
       <c r="A82" t="s" s="4">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="B82" t="s" s="4">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C82" t="s" s="4">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="D82" t="s" s="4">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="E82" s="5"/>
     </row>
     <row r="83" ht="15" customHeight="1">
       <c r="A83" t="s" s="4">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="B83" t="s" s="4">
-        <v>5</v>
+        <v>129</v>
       </c>
       <c r="C83" t="s" s="4">
-        <v>129</v>
-      </c>
-      <c r="D83" s="5"/>
+        <v>130</v>
+      </c>
+      <c r="D83" t="s" s="4">
+        <v>121</v>
+      </c>
       <c r="E83" s="5"/>
     </row>
     <row r="84" ht="15" customHeight="1">
       <c r="A84" t="s" s="4">
+        <v>78</v>
+      </c>
+      <c r="B84" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="C84" t="s" s="4">
+        <v>131</v>
+      </c>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+    </row>
+    <row r="85" ht="15" customHeight="1">
+      <c r="A85" t="s" s="4">
         <v>40</v>
       </c>
-      <c r="B84" t="s" s="4">
-        <v>130</v>
-      </c>
-      <c r="C84" t="s" s="4">
+      <c r="B85" t="s" s="4">
+        <v>132</v>
+      </c>
+      <c r="C85" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="D84" t="s" s="4">
-        <v>131</v>
-      </c>
-      <c r="E84" s="5"/>
+      <c r="D85" t="s" s="4">
+        <v>133</v>
+      </c>
+      <c r="E85" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A77:E77"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A71:E71"/>
+    <mergeCell ref="A31:E31"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A70:E70"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A46:E46"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A78:E78"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511806" footer="0.511806"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
add trucktype for orders tables.
</commit_message>
<xml_diff>
--- a/数据库/db.xlsx
+++ b/数据库/db.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="143">
   <si>
     <t>用户表-user</t>
   </si>
@@ -277,13 +277,22 @@
     <t>租车人对订单的评价</t>
   </si>
   <si>
+    <t>trucktype</t>
+  </si>
+  <si>
+    <t>汽车类型</t>
+  </si>
+  <si>
+    <t>(0, "小型货车"), (1, "大型货车"), (2, "小型平板"), (3, "中型平板"), (4, "大型平板"),</t>
+  </si>
+  <si>
     <t>status</t>
   </si>
   <si>
     <t>订单状态</t>
   </si>
   <si>
-    <t>0保存订单1预定订单2发起订单3订单被接受4完成订单5订单未完成结束</t>
+    <t>0系统选车订单1自主选车订单2长期订单3订单被接受4完成订单5订单未完成结束</t>
   </si>
   <si>
     <t>常用线路表-line</t>
@@ -356,12 +365,6 @@
   </si>
   <si>
     <t>长</t>
-  </si>
-  <si>
-    <t>汽车类型</t>
-  </si>
-  <si>
-    <t>(0, "小型货车"), (1, "大型货车"), (2, "小型平板"), (3, "中型平板"), (4, "大型平板"),</t>
   </si>
   <si>
     <t>modelinfo</t>
@@ -1606,7 +1609,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2253,7 +2256,7 @@
         <v>89</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D48" t="s" s="4">
         <v>79</v>
@@ -2263,102 +2266,106 @@
       </c>
     </row>
     <row r="49" ht="15" customHeight="1">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
+      <c r="A49" t="s" s="4">
+        <v>91</v>
+      </c>
+      <c r="B49" t="s" s="4">
+        <v>92</v>
+      </c>
+      <c r="C49" t="s" s="4">
+        <v>29</v>
+      </c>
+      <c r="D49" t="s" s="4">
+        <v>79</v>
+      </c>
+      <c r="E49" t="s" s="4">
+        <v>93</v>
+      </c>
     </row>
     <row r="50" ht="15" customHeight="1">
-      <c r="A50" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
     </row>
     <row r="51" ht="15" customHeight="1">
-      <c r="A51" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B51" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C51" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D51" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E51" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A51" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
     </row>
     <row r="52" ht="15" customHeight="1">
       <c r="A52" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>92</v>
+        <v>2</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D52" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E52" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E52" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="53" ht="15" customHeight="1">
       <c r="A53" t="s" s="4">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C53" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D53" t="s" s="4">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="E53" s="5"/>
     </row>
     <row r="54" ht="15" customHeight="1">
       <c r="A54" t="s" s="4">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C54" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D54" t="s" s="4">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="E54" s="5"/>
     </row>
     <row r="55" ht="15" customHeight="1">
       <c r="A55" t="s" s="4">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>69</v>
-      </c>
-      <c r="D55" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="D55" t="s" s="4">
+        <v>98</v>
+      </c>
       <c r="E55" s="5"/>
     </row>
     <row r="56" ht="15" customHeight="1">
       <c r="A56" t="s" s="4">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C56" t="s" s="4">
         <v>69</v>
@@ -2368,142 +2375,140 @@
     </row>
     <row r="57" ht="15" customHeight="1">
       <c r="A57" t="s" s="4">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
     </row>
     <row r="58" ht="15" customHeight="1">
       <c r="A58" t="s" s="4">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
     </row>
     <row r="59" ht="15" customHeight="1">
       <c r="A59" t="s" s="4">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
     </row>
     <row r="60" ht="15" customHeight="1">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
+      <c r="A60" t="s" s="4">
+        <v>86</v>
+      </c>
+      <c r="B60" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s" s="4">
+        <v>16</v>
+      </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
     </row>
     <row r="61" ht="15" customHeight="1">
-      <c r="A61" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
     </row>
     <row r="62" ht="15" customHeight="1">
-      <c r="A62" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B62" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C62" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D62" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E62" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A62" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
     </row>
     <row r="63" ht="15" customHeight="1">
       <c r="A63" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B63" t="s" s="4">
-        <v>103</v>
+        <v>2</v>
       </c>
       <c r="C63" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D63" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E63" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E63" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="64" ht="15" customHeight="1">
       <c r="A64" t="s" s="4">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="B64" t="s" s="4">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C64" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D64" t="s" s="4">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="E64" s="5"/>
     </row>
     <row r="65" ht="15" customHeight="1">
       <c r="A65" t="s" s="4">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="B65" t="s" s="4">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C65" t="s" s="4">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="D65" t="s" s="4">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="E65" s="5"/>
     </row>
     <row r="66" ht="15" customHeight="1">
       <c r="A66" t="s" s="4">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B66" t="s" s="4">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C66" t="s" s="4">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="D66" t="s" s="4">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="E66" s="5"/>
     </row>
     <row r="67" ht="15" customHeight="1">
       <c r="A67" t="s" s="4">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B67" t="s" s="4">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C67" t="s" s="4">
         <v>37</v>
@@ -2515,10 +2520,10 @@
     </row>
     <row r="68" ht="15" customHeight="1">
       <c r="A68" t="s" s="4">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B68" t="s" s="4">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C68" t="s" s="4">
         <v>37</v>
@@ -2530,10 +2535,10 @@
     </row>
     <row r="69" ht="15" customHeight="1">
       <c r="A69" t="s" s="4">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B69" t="s" s="4">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C69" t="s" s="4">
         <v>37</v>
@@ -2545,273 +2550,288 @@
     </row>
     <row r="70" ht="15" customHeight="1">
       <c r="A70" t="s" s="4">
-        <v>27</v>
+        <v>116</v>
       </c>
       <c r="B70" t="s" s="4">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C70" t="s" s="4">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="D70" t="s" s="4">
         <v>79</v>
       </c>
-      <c r="E70" t="s" s="4">
-        <v>116</v>
-      </c>
+      <c r="E70" s="5"/>
     </row>
     <row r="71" ht="15" customHeight="1">
       <c r="A71" t="s" s="4">
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="B71" t="s" s="4">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="C71" t="s" s="4">
-        <v>45</v>
-      </c>
-      <c r="D71" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="D71" t="s" s="4">
+        <v>79</v>
+      </c>
       <c r="E71" t="s" s="4">
-        <v>119</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1">
       <c r="A72" t="s" s="4">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="B72" t="s" s="4">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C72" t="s" s="4">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" t="s" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" ht="15" customHeight="1">
+      <c r="A73" t="s" s="4">
+        <v>86</v>
+      </c>
+      <c r="B73" t="s" s="4">
         <v>121</v>
       </c>
-    </row>
-    <row r="73" ht="15" customHeight="1">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
+      <c r="C73" t="s" s="4">
+        <v>69</v>
+      </c>
       <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
+      <c r="E73" t="s" s="4">
+        <v>122</v>
+      </c>
     </row>
     <row r="74" ht="15" customHeight="1">
-      <c r="A74" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
     </row>
     <row r="75" ht="15" customHeight="1">
-      <c r="A75" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B75" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C75" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D75" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E75" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A75" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
     </row>
     <row r="76" ht="15" customHeight="1">
       <c r="A76" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B76" t="s" s="4">
-        <v>123</v>
+        <v>2</v>
       </c>
       <c r="C76" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D76" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E76" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E76" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="77" ht="15" customHeight="1">
       <c r="A77" t="s" s="4">
+        <v>6</v>
+      </c>
+      <c r="B77" t="s" s="4">
         <v>124</v>
       </c>
-      <c r="B77" t="s" s="4">
-        <v>125</v>
-      </c>
       <c r="C77" t="s" s="4">
-        <v>16</v>
-      </c>
-      <c r="D77" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="D77" t="s" s="4">
+        <v>9</v>
+      </c>
       <c r="E77" s="5"/>
     </row>
     <row r="78" ht="15" customHeight="1">
       <c r="A78" t="s" s="4">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="B78" t="s" s="4">
         <v>126</v>
       </c>
       <c r="C78" t="s" s="4">
-        <v>37</v>
-      </c>
-      <c r="D78" t="s" s="4">
-        <v>79</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D78" s="5"/>
       <c r="E78" s="5"/>
     </row>
     <row r="79" ht="15" customHeight="1">
       <c r="A79" t="s" s="4">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s" s="4">
         <v>127</v>
       </c>
-      <c r="B79" t="s" s="4">
+      <c r="C79" t="s" s="4">
+        <v>37</v>
+      </c>
+      <c r="D79" t="s" s="4">
+        <v>79</v>
+      </c>
+      <c r="E79" s="5"/>
+    </row>
+    <row r="80" ht="15" customHeight="1">
+      <c r="A80" t="s" s="4">
         <v>128</v>
       </c>
-      <c r="C79" t="s" s="4">
+      <c r="B80" t="s" s="4">
+        <v>129</v>
+      </c>
+      <c r="C80" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="D79" t="s" s="4">
-        <v>129</v>
-      </c>
-      <c r="E79" s="5"/>
-    </row>
-    <row r="80" ht="15" customHeight="1">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
+      <c r="D80" t="s" s="4">
+        <v>130</v>
+      </c>
       <c r="E80" s="5"/>
     </row>
     <row r="81" ht="15" customHeight="1">
-      <c r="A81" t="s" s="2">
-        <v>130</v>
-      </c>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
     </row>
     <row r="82" ht="15" customHeight="1">
-      <c r="A82" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="B82" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="C82" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D82" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E82" t="s" s="4">
-        <v>5</v>
-      </c>
+      <c r="A82" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
     </row>
     <row r="83" ht="15" customHeight="1">
       <c r="A83" t="s" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B83" t="s" s="4">
-        <v>131</v>
+        <v>2</v>
       </c>
       <c r="C83" t="s" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D83" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="E83" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E83" t="s" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="84" ht="15" customHeight="1">
       <c r="A84" t="s" s="4">
+        <v>6</v>
+      </c>
+      <c r="B84" t="s" s="4">
         <v>132</v>
-      </c>
-      <c r="B84" t="s" s="4">
-        <v>133</v>
       </c>
       <c r="C84" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D84" t="s" s="4">
-        <v>134</v>
+        <v>9</v>
       </c>
       <c r="E84" s="5"/>
     </row>
     <row r="85" ht="15" customHeight="1">
       <c r="A85" t="s" s="4">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B85" t="s" s="4">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C85" t="s" s="4">
         <v>8</v>
       </c>
       <c r="D85" t="s" s="4">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E85" s="5"/>
     </row>
     <row r="86" ht="15" customHeight="1">
       <c r="A86" t="s" s="4">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="B86" t="s" s="4">
         <v>137</v>
       </c>
       <c r="C86" t="s" s="4">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="D86" t="s" s="4">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E86" s="5"/>
     </row>
     <row r="87" ht="15" customHeight="1">
       <c r="A87" t="s" s="4">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="B87" t="s" s="4">
-        <v>5</v>
+        <v>138</v>
       </c>
       <c r="C87" t="s" s="4">
         <v>139</v>
       </c>
-      <c r="D87" s="5"/>
+      <c r="D87" t="s" s="4">
+        <v>130</v>
+      </c>
       <c r="E87" s="5"/>
     </row>
     <row r="88" ht="15" customHeight="1">
       <c r="A88" t="s" s="4">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="C88" t="s" s="4">
+        <v>140</v>
+      </c>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+    </row>
+    <row r="89" ht="15" customHeight="1">
+      <c r="A89" t="s" s="4">
         <v>40</v>
       </c>
-      <c r="B88" t="s" s="4">
-        <v>140</v>
-      </c>
-      <c r="C88" t="s" s="4">
+      <c r="B89" t="s" s="4">
+        <v>141</v>
+      </c>
+      <c r="C89" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="D88" t="s" s="4">
-        <v>141</v>
-      </c>
-      <c r="E88" s="5"/>
+      <c r="D89" t="s" s="4">
+        <v>142</v>
+      </c>
+      <c r="E89" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="A74:E74"/>
+    <mergeCell ref="A82:E82"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A75:E75"/>
     <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A81:E81"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511806" footer="0.511806"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
add a choice to the status of order
</commit_message>
<xml_diff>
--- a/数据库/db.xlsx
+++ b/数据库/db.xlsx
@@ -292,7 +292,7 @@
     <t>订单状态</t>
   </si>
   <si>
-    <t>0系统选车订单1自主选车订单2长期订单3订单被接受4完成订单5订单未完成结束</t>
+    <t>0系统选车订单1自主选车订单2长期订单3订单被接受4完成订单5订单未完成结束6预约订单</t>
   </si>
   <si>
     <t>常用线路表-line</t>
@@ -2824,14 +2824,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A75:E75"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A1:E1"/>
     <mergeCell ref="A82:E82"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="A62:E62"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A75:E75"/>
-    <mergeCell ref="A32:E32"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511806" footer="0.511806"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>